<commit_message>
ajouter le rapport le livrable
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OpenClassRooms\Livrable\projet 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3764EF7A-30F7-45F1-A227-A576B1CEC7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7C2ED7-407B-4FA1-98C4-E7E9D204DA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,10 +69,6 @@
     <t>Balise HTML avec langue</t>
   </si>
   <si>
-    <t>L'attribut lang permet aux robots de mieux localiser le site
-L’identification de la langue de la page ou des éléments de page permet aux lecteurs d’écran de lire le contenu dans la langue appropriée. Il facilite également la traduction automatique du contenu.</t>
-  </si>
-  <si>
     <t>Mettre un attribut lang valide</t>
   </si>
   <si>
@@ -85,17 +81,10 @@
     <t>plusieurs liens menent à une même page ce qui peut desservir l'indexation</t>
   </si>
   <si>
-    <t xml:space="preserve"> combinez les liens redondants en un seul lien et supprimez tout texte redondant ou texte alternatif (par exemple, si une image de produit et le nom du produit se trouvent dans le même lien, l’image peut généralement recevoir alt=" »).</t>
-  </si>
-  <si>
     <t>meta description vide</t>
   </si>
   <si>
     <t>Remplir la méta description</t>
-  </si>
-  <si>
-    <t>La description servira à google pour l'afficher sur
- la page de recherche</t>
   </si>
   <si>
     <t>Format d'image BMP</t>
@@ -135,73 +124,82 @@
   <si>
     <t>Si les couleurs de texte et de fond sont trop similaire alors on peut
  avoir du mal à lire le texte Un contraste adéquat du texte est nécessaire pour tous les utilisateurs, en particulier les utilisateurs malvoyants.  Les éléments doivent avoir un contraste de couleurs suffisant</t>
+  </si>
+  <si>
+    <t>Absence de la totalité des balises
+ sémantiques, La page doit contenir des balises sémantiques (nav, main,,,,)</t>
+  </si>
+  <si>
+    <t>Utiliser toute les balises sémantiques</t>
+  </si>
+  <si>
+    <t>Elles permettent de structurer la page avec un en-tête (header),  une zone de navigation (nav),une zone de contenu principale (main) et un pied de page (footer)</t>
+  </si>
+  <si>
+    <t>Mettre en place les balise sémantiques 
+manquantes</t>
+  </si>
+  <si>
+    <t>Code html css, js non minifiés</t>
+  </si>
+  <si>
+    <t>Afin de réduire le poids de la page, il est conseillé de minifier le code</t>
+  </si>
+  <si>
+    <t>Un code non minifié alourdit la page et ralentit son chargement</t>
+  </si>
+  <si>
+    <t>Minifier les codes présents</t>
+  </si>
+  <si>
+    <t>Détection de pratiques "black hat". Des mot clés en blanc
+ sur font blanc dans le header</t>
+  </si>
+  <si>
+    <t>Risque important de blacklistage par Google</t>
+  </si>
+  <si>
+    <t>Supprimer ces mots clés cachés</t>
+  </si>
+  <si>
+    <t>Les Urls des pages doient données une idée sur le continu de la page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Url de la page2 n'a pas un sens sémentique </t>
+  </si>
+  <si>
+    <t>Le niveau de hiérarchisation de Heading non respecté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le niveau de hiérarchisation de Heading respecter H2 sous H1 et H3 sous H2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corriger le lien pour avoir un url simple que donne une vue sur le contenue de la page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corriger les heading on mettrant H1 -&gt; H2 -&gt;H3 </t>
+  </si>
+  <si>
+    <t>L'attribut lang permet aux robots de mieux localiser le site
+L’identification de la langue de la page ou des éléments de page permet aux internautes de lire le contenu dans la langue appropriée. Il facilite également la traduction automatique du contenu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> combiner les liens redondants en un seul lien et supprimer tout texte redondant ou texte alternatif (par exemple, si une image de produit et le nom du produit se trouvent dans le même lien, l’image peut généralement recevoir alt=" »).</t>
+  </si>
+  <si>
+    <t>La description servira à google pour l'afficher sur la page de recherche</t>
   </si>
   <si>
     <t xml:space="preserve">Changer les couleurs pour avoir un meilleur
  contraste et donc une meilleure lisibilité
 Augmentez le contraste entre la couleur de premier plan (texte) et la couleur d’arrière-plan. Un texte volumineux (plus grand que 18 points ou 14 points en gras) ne nécessite pas autant de contraste que le texte plus petit.
-L’algorithme... en anglais
 </t>
   </si>
   <si>
-    <t>Absence de la totalité des balises
- sémantiques, La page doit contenir des balises sémantiques (nav, main,,,,)</t>
-  </si>
-  <si>
-    <t>Utiliser toute les balises sémantiques</t>
-  </si>
-  <si>
-    <t>Elles permettent de structurer la page avec un en-tête (header),  une zone de navigation (nav),une zone de contenu principale (main) et un pied de page (footer)</t>
-  </si>
-  <si>
-    <t>Mettre en place les balise sémantiques 
-manquantes</t>
-  </si>
-  <si>
-    <t>Code html css, js non minifiés</t>
-  </si>
-  <si>
-    <t>Afin de réduire le poids de la page, il est conseillé de minifier le code</t>
-  </si>
-  <si>
-    <t>Un code non minifié alourdit la page et ralentit son chargement</t>
-  </si>
-  <si>
-    <t>Minifier les codes présents</t>
-  </si>
-  <si>
-    <t>Détection de pratiques "black hat". Des mot clés en blanc
- sur font blanc dans le header</t>
-  </si>
-  <si>
-    <t>Ne pas chercher à tromper les moteurs de recherche, les pratiques black hat sont à prohiber + Tout ce qui est invisible à l'écran doit réellement être invisible.</t>
-  </si>
-  <si>
-    <t>Risque important de blacklistage par Google</t>
-  </si>
-  <si>
-    <t>Supprimer ces mots clés cachés</t>
-  </si>
-  <si>
-    <t>Les Urls des pages doient données une idée sur le continu de la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Url de la page2 n'a pas un sens sémentique </t>
-  </si>
-  <si>
-    <t>Risque mal indexation par Google</t>
-  </si>
-  <si>
-    <t>Le niveau de hiérarchisation de Heading non respecté</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le niveau de hiérarchisation de Heading respecter H2 sous H1 et H3 sous H2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corriger le lien pour avoir un url simple que donne une vue sur le contenue de la page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corriger les heading on mettrant H1 -&gt; H2 -&gt;H3 </t>
+    <t>Ne pas chercher à tromper les moteurs de recherche, les pratiques black hat sont à prohiber, Tout ce qui est invisible à l'écran doit réellement être invisible.</t>
+  </si>
+  <si>
+    <t>Risque mauvaise indexation par Google</t>
   </si>
 </sst>
 </file>
@@ -335,42 +333,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -378,16 +346,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -619,10 +608,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="A1:F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -676,243 +668,243 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:26" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="69" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="C4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="69" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="5" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="D5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="E6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="B7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="C7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="D7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="E7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:26" ht="69" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="B8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="124.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="B10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="C10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="D10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="69" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="11" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="B11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="12" spans="1:26" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="B12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="D12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="69" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+    <row r="13" spans="1:26" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="18" t="s">
+      <c r="B13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="D13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1921,6 +1913,6 @@
     <hyperlink ref="F13" r:id="rId13" xr:uid="{F8A6EAED-6201-44F8-87FC-EE513AE6AE0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId14"/>
+  <pageSetup scale="70" orientation="landscape" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>